<commit_message>
Added extra document, corrected algorithm analysis sheet
</commit_message>
<xml_diff>
--- a/Analisis Empirico Selection Insertion Sorts.xlsx
+++ b/Analisis Empirico Selection Insertion Sorts.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="19155" windowHeight="8250"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="19155" windowHeight="8250" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -215,67 +215,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>509000</c:v>
+                  <c:v>4848000000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2018000</c:v>
+                  <c:v>38592000000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4527000</c:v>
+                  <c:v>130032000000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8036000</c:v>
+                  <c:v>307968000000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>12545000</c:v>
+                  <c:v>601200000000</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>18054000</c:v>
+                  <c:v>1038528000000</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>32072000</c:v>
+                  <c:v>2460672000000</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>40581000</c:v>
+                  <c:v>3503088000000</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>50090000</c:v>
+                  <c:v>4804800000000</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>60599000</c:v>
+                  <c:v>6394608000000</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>72108000</c:v>
+                  <c:v>8301312000000</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>84617000</c:v>
+                  <c:v>10553712000000</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>98126000</c:v>
+                  <c:v>13180608000000</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>112635000</c:v>
+                  <c:v>16210800000000</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>128144000</c:v>
+                  <c:v>19673088000000</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>144653000</c:v>
+                  <c:v>23596272000000</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>162162000</c:v>
+                  <c:v>28009152000000</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>180671000</c:v>
+                  <c:v>32940528000000</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>200180000</c:v>
+                  <c:v>38419200000000</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>220689000</c:v>
+                  <c:v>44473968000000</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>242198000</c:v>
+                  <c:v>51133632000000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -378,67 +378,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>1104000</c:v>
+                  <c:v>6399360000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4408000</c:v>
+                  <c:v>51198720000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9912000</c:v>
+                  <c:v>172798080000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>17616000</c:v>
+                  <c:v>409597440000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>27520000</c:v>
+                  <c:v>799996800000</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>39624000</c:v>
+                  <c:v>1382396160000</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>70432000</c:v>
+                  <c:v>3276794880000</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>89136000</c:v>
+                  <c:v>4665594240000</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>110040000</c:v>
+                  <c:v>6399993600000</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>133144000</c:v>
+                  <c:v>8518392960000</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>158448000</c:v>
+                  <c:v>11059192320000</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>185952000</c:v>
+                  <c:v>14060791680000</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>215656000</c:v>
+                  <c:v>17561591040000</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>247560000</c:v>
+                  <c:v>21599990400000</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>281664000</c:v>
+                  <c:v>26214389760000</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>317968000</c:v>
+                  <c:v>31443189120000</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>356472000</c:v>
+                  <c:v>37324788480000</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>397176000</c:v>
+                  <c:v>43897587840000</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>440080000</c:v>
+                  <c:v>51199987200000</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>485184000</c:v>
+                  <c:v>59270386560000</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>532488000</c:v>
+                  <c:v>68147185920000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -455,11 +455,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="95538176"/>
-        <c:axId val="95544448"/>
+        <c:axId val="94878720"/>
+        <c:axId val="94884992"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="95538176"/>
+        <c:axId val="94878720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -488,7 +488,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95544448"/>
+        <c:crossAx val="94884992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -496,7 +496,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="95544448"/>
+        <c:axId val="94884992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -526,7 +526,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95538176"/>
+        <c:crossAx val="94878720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -664,67 +664,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>316200</c:v>
+                  <c:v>2348250000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1252400</c:v>
+                  <c:v>18693000000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2808600</c:v>
+                  <c:v>62984250000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4984800</c:v>
+                  <c:v>149172000000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7781000</c:v>
+                  <c:v>291206250000</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>11197200</c:v>
+                  <c:v>503037000000</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>19889600</c:v>
+                  <c:v>1191888000000</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>25165800</c:v>
+                  <c:v>1696808250000</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>31062000</c:v>
+                  <c:v>2327325000000</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>37578200</c:v>
+                  <c:v>3097388250000</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>44714400</c:v>
+                  <c:v>4020948000000</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>52470600</c:v>
+                  <c:v>5111954250000</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>60846800</c:v>
+                  <c:v>6384357000000</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>69843000</c:v>
+                  <c:v>7852106250000</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>79459200</c:v>
+                  <c:v>9529152000000</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>89695400</c:v>
+                  <c:v>11429444250000</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>100551600</c:v>
+                  <c:v>13566933000000</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>112027800</c:v>
+                  <c:v>15955568250000</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>124124000</c:v>
+                  <c:v>18609300000000</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>136840200</c:v>
+                  <c:v>21542078250000</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>150176400</c:v>
+                  <c:v>24767853000000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -827,67 +827,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>981700</c:v>
+                  <c:v>3629637000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3923400</c:v>
+                  <c:v>29039274000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8825100</c:v>
+                  <c:v>98008911000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>15686800</c:v>
+                  <c:v>232318548000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>24508500</c:v>
+                  <c:v>453748185000</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>35290200</c:v>
+                  <c:v>784077822000</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>62733600</c:v>
+                  <c:v>1858557096000</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>79395300</c:v>
+                  <c:v>2646266733000</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>98017000</c:v>
+                  <c:v>3629996370000</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>118598700</c:v>
+                  <c:v>4831526007000</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>141140400</c:v>
+                  <c:v>6272635644000</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>165642100</c:v>
+                  <c:v>7975105281000</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>192103800</c:v>
+                  <c:v>9960714918000</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>220525500</c:v>
+                  <c:v>12251244555000</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>250907200</c:v>
+                  <c:v>14868474192000</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>283248900</c:v>
+                  <c:v>17834183829000</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>317550600</c:v>
+                  <c:v>21170153466000</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>353812300</c:v>
+                  <c:v>24898163103000</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>392034000</c:v>
+                  <c:v>29039992740000</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>432215700</c:v>
+                  <c:v>33617422377000</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>474357400</c:v>
+                  <c:v>38652232014000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -904,11 +904,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="97200384"/>
-        <c:axId val="97202560"/>
+        <c:axId val="97523968"/>
+        <c:axId val="97530240"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="97200384"/>
+        <c:axId val="97523968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -930,13 +930,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="97202560"/>
+        <c:crossAx val="97530240"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -944,7 +945,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="97202560"/>
+        <c:axId val="97530240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -967,19 +968,21 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="97200384"/>
+        <c:crossAx val="97523968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1110,67 +1113,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>663500</c:v>
+                  <c:v>14392500000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2627000</c:v>
+                  <c:v>114570000000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5890500</c:v>
+                  <c:v>386032500000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10454000</c:v>
+                  <c:v>914280000000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16317500</c:v>
+                  <c:v>1784812500000</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>23481000</c:v>
+                  <c:v>3083130000000</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>41708000</c:v>
+                  <c:v>7305120000000</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>52771500</c:v>
+                  <c:v>10399792500000</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>65135000</c:v>
+                  <c:v>14264250000000</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>78798500</c:v>
+                  <c:v>18983992500000</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>93762000</c:v>
+                  <c:v>24644520000000</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>110025500</c:v>
+                  <c:v>31331332500000</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>127589000</c:v>
+                  <c:v>39129930000000</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>146452500</c:v>
+                  <c:v>48125812500000</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>166616000</c:v>
+                  <c:v>58404480000000</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>188079500</c:v>
+                  <c:v>70051432500000</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>210843000</c:v>
+                  <c:v>83152170000000</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>234906500</c:v>
+                  <c:v>97792192500000</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>260270000</c:v>
+                  <c:v>114057000000000</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>286933500</c:v>
+                  <c:v>132032092500000</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>314897000</c:v>
+                  <c:v>151802970000000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1273,67 +1276,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>1904500</c:v>
+                  <c:v>14948505000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7609000</c:v>
+                  <c:v>119597010000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>17113500</c:v>
+                  <c:v>403645515000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>30418000</c:v>
+                  <c:v>956794020000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>47522500</c:v>
+                  <c:v>1868742525000</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>68427000</c:v>
+                  <c:v>3229191030000</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>121636000</c:v>
+                  <c:v>7654388040000</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>153940500</c:v>
+                  <c:v>10898536545000</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>190045000</c:v>
+                  <c:v>14949985050000</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>229949500</c:v>
+                  <c:v>19898433555000</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>273654000</c:v>
+                  <c:v>25833582060000</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>321158500</c:v>
+                  <c:v>32845130565000</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>372463000</c:v>
+                  <c:v>41022779070000</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>427567500</c:v>
+                  <c:v>50456227575000</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>486472000</c:v>
+                  <c:v>61235176080000</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>549176500</c:v>
+                  <c:v>73449324585000</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>615681000</c:v>
+                  <c:v>87188373090000</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>685985500</c:v>
+                  <c:v>102542021595000</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>760090000</c:v>
+                  <c:v>119599970100000</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>837994500</c:v>
+                  <c:v>138451918605000</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>919699000</c:v>
+                  <c:v>159187567110000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1350,11 +1353,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="97244672"/>
-        <c:axId val="97246592"/>
+        <c:axId val="97576448"/>
+        <c:axId val="97578368"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="97244672"/>
+        <c:axId val="97576448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1376,13 +1379,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="97246592"/>
+        <c:crossAx val="97578368"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1390,7 +1394,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="97246592"/>
+        <c:axId val="97578368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1413,19 +1417,21 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="97244672"/>
+        <c:crossAx val="97576448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1556,67 +1562,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>267800</c:v>
+                  <c:v>1688720000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1055600</c:v>
+                  <c:v>13442880000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2363400</c:v>
+                  <c:v>45294480000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4191200</c:v>
+                  <c:v>107275520000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6539000</c:v>
+                  <c:v>209418000000</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9406800</c:v>
+                  <c:v>361753920000</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>16702400</c:v>
+                  <c:v>857134080000</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>21130200</c:v>
+                  <c:v>1220242320000</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>26078000</c:v>
+                  <c:v>1673672000000</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>31545800</c:v>
+                  <c:v>2227455120000</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>37533600</c:v>
+                  <c:v>2891623680000</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44041400</c:v>
+                  <c:v>3676209680000</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>51069200</c:v>
+                  <c:v>4591245120000</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>58617000</c:v>
+                  <c:v>5646762000000</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>66684800</c:v>
+                  <c:v>6852792320000</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>75272600</c:v>
+                  <c:v>8219368080000</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>84380400</c:v>
+                  <c:v>9756521280000</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>94008200</c:v>
+                  <c:v>11474283920000</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>104156000</c:v>
+                  <c:v>13382688000000</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>114823800</c:v>
+                  <c:v>15491765520000</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>126011600</c:v>
+                  <c:v>17811548480000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1719,67 +1725,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>761800</c:v>
+                  <c:v>2391760800</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3043600</c:v>
+                  <c:v>19135521600</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6845400</c:v>
+                  <c:v>64583282400</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12167200</c:v>
+                  <c:v>153087043200</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>19009000</c:v>
+                  <c:v>298998804000</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>27370800</c:v>
+                  <c:v>516670564800</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>48654400</c:v>
+                  <c:v>1224702086400</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>61576200</c:v>
+                  <c:v>1743765847200</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>76018000</c:v>
+                  <c:v>2391997608000</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>91979800</c:v>
+                  <c:v>3183749368800</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>109461600</c:v>
+                  <c:v>4133373129600</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>128463400</c:v>
+                  <c:v>5255220890400</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>148985200</c:v>
+                  <c:v>6563644651200</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>171027000</c:v>
+                  <c:v>8072996412000</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>194588800</c:v>
+                  <c:v>9797628172800</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>219670600</c:v>
+                  <c:v>11751891933600</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>246272400</c:v>
+                  <c:v>13950139694400</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>274394200</c:v>
+                  <c:v>16406723455200</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>304036000</c:v>
+                  <c:v>19135995216000</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>335197800</c:v>
+                  <c:v>22152306976800</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>367879600</c:v>
+                  <c:v>25470010737600</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1796,11 +1802,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="97921280"/>
-        <c:axId val="97923456"/>
+        <c:axId val="97399552"/>
+        <c:axId val="97401472"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="97921280"/>
+        <c:axId val="97399552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1836,7 +1842,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="97923456"/>
+        <c:crossAx val="97401472"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1844,7 +1850,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="97923456"/>
+        <c:axId val="97401472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1867,19 +1873,21 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="97921280"/>
+        <c:crossAx val="97399552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2002,67 +2010,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>398100</c:v>
+                  <c:v>3799620000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1576200</c:v>
+                  <c:v>30246480000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3534300</c:v>
+                  <c:v>101912580000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6272400</c:v>
+                  <c:v>241369920000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9790500</c:v>
+                  <c:v>471190500000</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>14088600</c:v>
+                  <c:v>813946320000</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>25024800</c:v>
+                  <c:v>1928551680000</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>31662900</c:v>
+                  <c:v>2745545220000</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>39081000</c:v>
+                  <c:v>3765762000000</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>47279100</c:v>
+                  <c:v>5011774020000</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>56257200</c:v>
+                  <c:v>6506153280000</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>66015300</c:v>
+                  <c:v>8271471780000</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>76553400</c:v>
+                  <c:v>10330301520000</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>87871500</c:v>
+                  <c:v>12705214500000</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>99969600</c:v>
+                  <c:v>15418782720000</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>112847700</c:v>
+                  <c:v>18493578180000</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>126505800</c:v>
+                  <c:v>21952172880000</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>140943900</c:v>
+                  <c:v>25817138820000</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>156162000</c:v>
+                  <c:v>30111048000000</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>172160100</c:v>
+                  <c:v>34856472420000</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>188938200</c:v>
+                  <c:v>40075984080000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2157,67 +2165,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>1142400</c:v>
+                  <c:v>5381461800</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4564800</c:v>
+                  <c:v>43054923600</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10267200</c:v>
+                  <c:v>145312385400</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>18249600</c:v>
+                  <c:v>344445847200</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>28512000</c:v>
+                  <c:v>672747309000</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>41054400</c:v>
+                  <c:v>1162508770800</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>72979200</c:v>
+                  <c:v>2755579694400</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>92361600</c:v>
+                  <c:v>3923473156200</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>114024000</c:v>
+                  <c:v>5381994618000</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>137966400</c:v>
+                  <c:v>7163436079800</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>164188800</c:v>
+                  <c:v>9300089541600</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>192691200</c:v>
+                  <c:v>11824247003400</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>223473600</c:v>
+                  <c:v>14768200465200</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>256536000</c:v>
+                  <c:v>18164241927000</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>291878400</c:v>
+                  <c:v>22044663388800</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>329500800</c:v>
+                  <c:v>26441756850600</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>369403200</c:v>
+                  <c:v>31387814312400</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>411585600</c:v>
+                  <c:v>36915127774200</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>456048000</c:v>
+                  <c:v>43055989236000</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>502790400</c:v>
+                  <c:v>49842690697800</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>551812800</c:v>
+                  <c:v>57307524159600</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2234,11 +2242,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="97973376"/>
-        <c:axId val="97975296"/>
+        <c:axId val="97449088"/>
+        <c:axId val="97451008"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="97973376"/>
+        <c:axId val="97449088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2260,13 +2268,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="97975296"/>
+        <c:crossAx val="97451008"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2274,7 +2283,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="97975296"/>
+        <c:axId val="97451008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2297,19 +2306,21 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="97973376"/>
+        <c:crossAx val="97449088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2328,16 +2339,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>219074</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>147637</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>533399</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>609599</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>314324</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2788,8 +2799,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2823,12 +2834,12 @@
         <v>100</v>
       </c>
       <c r="B2">
-        <f xml:space="preserve"> A2 * (10 + 4*10 + 10 + 3*10 + A2*(2*10 + 10 + 10 + 10))</f>
-        <v>509000</v>
+        <f>A2*(4*10 + 10 + 3*10 +4*10)*(3*10 + 2*10 + 10 + 2*10)*((A2)*(A2+1))/2</f>
+        <v>4848000000</v>
       </c>
       <c r="C2">
-        <f>A2 * (2*10 + 10 + 10 + A2 * (2 * 10 + 3 * 10 + 6 * 10))</f>
-        <v>1104000</v>
+        <f xml:space="preserve"> A2 *(3*10 + 10 + 4*10)*(4*10 + 2*10 + 4*10 + 6*10)*((A2 - 1)*(A2 + 1))/2</f>
+        <v>6399360000</v>
       </c>
       <c r="H2" t="s">
         <v>5</v>
@@ -2842,12 +2853,12 @@
         <v>200</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:B22" si="0" xml:space="preserve"> A3 * (10 + 4*10 + 10 + 3*10 + A3*(2*10 + 10 + 10 + 10))</f>
-        <v>2018000</v>
+        <f t="shared" ref="B3:B22" si="0">A3*(4*10 + 10 + 3*10 +4*10)*(3*10 + 2*10 + 10 + 2*10)*((A3)*(A3+1))/2</f>
+        <v>38592000000</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C22" si="1">A3 * (2*10 + 10 + 10 + A3 * (2 * 10 + 3 * 10 + 6 * 10))</f>
-        <v>4408000</v>
+        <f t="shared" ref="C3:C22" si="1" xml:space="preserve"> A3 *(3*10 + 10 + 4*10)*(4*10 + 2*10 + 4*10 + 6*10)*((A3 - 1)*(A3 + 1))/2</f>
+        <v>51198720000</v>
       </c>
       <c r="H3" t="s">
         <v>3</v>
@@ -2862,11 +2873,11 @@
       </c>
       <c r="B4">
         <f t="shared" si="0"/>
-        <v>4527000</v>
+        <v>130032000000</v>
       </c>
       <c r="C4">
         <f t="shared" si="1"/>
-        <v>9912000</v>
+        <v>172798080000</v>
       </c>
       <c r="H4" t="s">
         <v>6</v>
@@ -2881,11 +2892,11 @@
       </c>
       <c r="B5">
         <f t="shared" si="0"/>
-        <v>8036000</v>
+        <v>307968000000</v>
       </c>
       <c r="C5">
         <f t="shared" si="1"/>
-        <v>17616000</v>
+        <v>409597440000</v>
       </c>
       <c r="H5" t="s">
         <v>7</v>
@@ -2900,11 +2911,11 @@
       </c>
       <c r="B6">
         <f t="shared" si="0"/>
-        <v>12545000</v>
+        <v>601200000000</v>
       </c>
       <c r="C6">
         <f t="shared" si="1"/>
-        <v>27520000</v>
+        <v>799996800000</v>
       </c>
       <c r="H6" t="s">
         <v>8</v>
@@ -2919,11 +2930,11 @@
       </c>
       <c r="B7">
         <f t="shared" si="0"/>
-        <v>18054000</v>
+        <v>1038528000000</v>
       </c>
       <c r="C7">
         <f t="shared" si="1"/>
-        <v>39624000</v>
+        <v>1382396160000</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -2932,11 +2943,11 @@
       </c>
       <c r="B8">
         <f t="shared" si="0"/>
-        <v>32072000</v>
+        <v>2460672000000</v>
       </c>
       <c r="C8">
         <f t="shared" si="1"/>
-        <v>70432000</v>
+        <v>3276794880000</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -2945,11 +2956,11 @@
       </c>
       <c r="B9">
         <f t="shared" si="0"/>
-        <v>40581000</v>
+        <v>3503088000000</v>
       </c>
       <c r="C9">
         <f t="shared" si="1"/>
-        <v>89136000</v>
+        <v>4665594240000</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -2957,12 +2968,12 @@
         <v>1000</v>
       </c>
       <c r="B10">
-        <f xml:space="preserve"> A10 * (10 + 4*10 + 10 + 3*10 + A10*(2*10 + 10 + 10 + 10))</f>
-        <v>50090000</v>
+        <f t="shared" si="0"/>
+        <v>4804800000000</v>
       </c>
       <c r="C10">
         <f t="shared" si="1"/>
-        <v>110040000</v>
+        <v>6399993600000</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -2971,11 +2982,11 @@
       </c>
       <c r="B11">
         <f t="shared" si="0"/>
-        <v>60599000</v>
+        <v>6394608000000</v>
       </c>
       <c r="C11">
         <f t="shared" si="1"/>
-        <v>133144000</v>
+        <v>8518392960000</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -2984,11 +2995,11 @@
       </c>
       <c r="B12">
         <f t="shared" si="0"/>
-        <v>72108000</v>
+        <v>8301312000000</v>
       </c>
       <c r="C12">
         <f t="shared" si="1"/>
-        <v>158448000</v>
+        <v>11059192320000</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -2997,11 +3008,11 @@
       </c>
       <c r="B13">
         <f t="shared" si="0"/>
-        <v>84617000</v>
+        <v>10553712000000</v>
       </c>
       <c r="C13">
         <f t="shared" si="1"/>
-        <v>185952000</v>
+        <v>14060791680000</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -3010,11 +3021,11 @@
       </c>
       <c r="B14">
         <f t="shared" si="0"/>
-        <v>98126000</v>
+        <v>13180608000000</v>
       </c>
       <c r="C14">
         <f t="shared" si="1"/>
-        <v>215656000</v>
+        <v>17561591040000</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -3023,11 +3034,11 @@
       </c>
       <c r="B15">
         <f t="shared" si="0"/>
-        <v>112635000</v>
+        <v>16210800000000</v>
       </c>
       <c r="C15">
         <f t="shared" si="1"/>
-        <v>247560000</v>
+        <v>21599990400000</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -3036,11 +3047,11 @@
       </c>
       <c r="B16">
         <f t="shared" si="0"/>
-        <v>128144000</v>
+        <v>19673088000000</v>
       </c>
       <c r="C16">
         <f t="shared" si="1"/>
-        <v>281664000</v>
+        <v>26214389760000</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -3049,11 +3060,11 @@
       </c>
       <c r="B17">
         <f t="shared" si="0"/>
-        <v>144653000</v>
+        <v>23596272000000</v>
       </c>
       <c r="C17">
         <f t="shared" si="1"/>
-        <v>317968000</v>
+        <v>31443189120000</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -3062,11 +3073,11 @@
       </c>
       <c r="B18">
         <f t="shared" si="0"/>
-        <v>162162000</v>
+        <v>28009152000000</v>
       </c>
       <c r="C18">
         <f t="shared" si="1"/>
-        <v>356472000</v>
+        <v>37324788480000</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -3075,11 +3086,11 @@
       </c>
       <c r="B19">
         <f t="shared" si="0"/>
-        <v>180671000</v>
+        <v>32940528000000</v>
       </c>
       <c r="C19">
         <f t="shared" si="1"/>
-        <v>397176000</v>
+        <v>43897587840000</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -3088,11 +3099,11 @@
       </c>
       <c r="B20">
         <f t="shared" si="0"/>
-        <v>200180000</v>
+        <v>38419200000000</v>
       </c>
       <c r="C20">
         <f t="shared" si="1"/>
-        <v>440080000</v>
+        <v>51199987200000</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -3101,11 +3112,11 @@
       </c>
       <c r="B21">
         <f t="shared" si="0"/>
-        <v>220689000</v>
+        <v>44473968000000</v>
       </c>
       <c r="C21">
         <f t="shared" si="1"/>
-        <v>485184000</v>
+        <v>59270386560000</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -3114,11 +3125,11 @@
       </c>
       <c r="B22">
         <f t="shared" si="0"/>
-        <v>242198000</v>
+        <v>51133632000000</v>
       </c>
       <c r="C22">
         <f t="shared" si="1"/>
-        <v>532488000</v>
+        <v>68147185920000</v>
       </c>
     </row>
   </sheetData>
@@ -3131,8 +3142,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A22"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3165,12 +3176,12 @@
         <v>100</v>
       </c>
       <c r="B2">
-        <f xml:space="preserve"> A2 * (1 + 4*2 + 8 + 3*15 + A2*(2*1 + 2 + 12 + 15))</f>
-        <v>316200</v>
+        <f>A2*(4*2 + 1 + 3*8 +4*15)*(3*2 + 2*1 + 12 + 2*15)*((A2)*(A2+1))/2</f>
+        <v>2348250000</v>
       </c>
       <c r="C2">
-        <f>A2 * (2*2 + 1 + 12 + A2 * (2 * 1 + 3 * 2 + 6 * 15))</f>
-        <v>981700</v>
+        <f xml:space="preserve"> A2 *(3*2 + 1 + 4*12)*(4*2 + 2*1 + 4*8 + 6*15)*((A2 - 1)*(A2 + 1))/2</f>
+        <v>3629637000</v>
       </c>
       <c r="H2" t="s">
         <v>5</v>
@@ -3184,12 +3195,12 @@
         <v>200</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:B22" si="0" xml:space="preserve"> A3 * (1 + 4*2 + 8 + 3*15 + A3*(2*1 + 2 + 12 + 15))</f>
-        <v>1252400</v>
+        <f t="shared" ref="B3:B22" si="0">A3*(4*2 + 1 + 3*8 +4*15)*(3*2 + 2*1 + 12 + 2*15)*((A3)*(A3+1))/2</f>
+        <v>18693000000</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C22" si="1">A3 * (2*2 + 1 + 12 + A3 * (2 * 1 + 3 * 2 + 6 * 15))</f>
-        <v>3923400</v>
+        <f t="shared" ref="C3:C22" si="1" xml:space="preserve"> A3 *(3*2 + 1 + 4*12)*(4*2 + 2*1 + 4*8 + 6*15)*((A3 - 1)*(A3 + 1))/2</f>
+        <v>29039274000</v>
       </c>
       <c r="H3" t="s">
         <v>3</v>
@@ -3204,11 +3215,11 @@
       </c>
       <c r="B4">
         <f t="shared" si="0"/>
-        <v>2808600</v>
+        <v>62984250000</v>
       </c>
       <c r="C4">
         <f t="shared" si="1"/>
-        <v>8825100</v>
+        <v>98008911000</v>
       </c>
       <c r="H4" t="s">
         <v>6</v>
@@ -3223,11 +3234,11 @@
       </c>
       <c r="B5">
         <f t="shared" si="0"/>
-        <v>4984800</v>
+        <v>149172000000</v>
       </c>
       <c r="C5">
         <f t="shared" si="1"/>
-        <v>15686800</v>
+        <v>232318548000</v>
       </c>
       <c r="H5" t="s">
         <v>7</v>
@@ -3242,11 +3253,11 @@
       </c>
       <c r="B6">
         <f t="shared" si="0"/>
-        <v>7781000</v>
+        <v>291206250000</v>
       </c>
       <c r="C6">
         <f t="shared" si="1"/>
-        <v>24508500</v>
+        <v>453748185000</v>
       </c>
       <c r="H6" t="s">
         <v>8</v>
@@ -3261,11 +3272,11 @@
       </c>
       <c r="B7">
         <f t="shared" si="0"/>
-        <v>11197200</v>
+        <v>503037000000</v>
       </c>
       <c r="C7">
         <f t="shared" si="1"/>
-        <v>35290200</v>
+        <v>784077822000</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -3274,11 +3285,11 @@
       </c>
       <c r="B8">
         <f t="shared" si="0"/>
-        <v>19889600</v>
+        <v>1191888000000</v>
       </c>
       <c r="C8">
         <f t="shared" si="1"/>
-        <v>62733600</v>
+        <v>1858557096000</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -3287,11 +3298,11 @@
       </c>
       <c r="B9">
         <f t="shared" si="0"/>
-        <v>25165800</v>
+        <v>1696808250000</v>
       </c>
       <c r="C9">
         <f t="shared" si="1"/>
-        <v>79395300</v>
+        <v>2646266733000</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -3300,11 +3311,11 @@
       </c>
       <c r="B10">
         <f t="shared" si="0"/>
-        <v>31062000</v>
+        <v>2327325000000</v>
       </c>
       <c r="C10">
         <f t="shared" si="1"/>
-        <v>98017000</v>
+        <v>3629996370000</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -3313,11 +3324,11 @@
       </c>
       <c r="B11">
         <f t="shared" si="0"/>
-        <v>37578200</v>
+        <v>3097388250000</v>
       </c>
       <c r="C11">
         <f t="shared" si="1"/>
-        <v>118598700</v>
+        <v>4831526007000</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -3326,11 +3337,11 @@
       </c>
       <c r="B12">
         <f t="shared" si="0"/>
-        <v>44714400</v>
+        <v>4020948000000</v>
       </c>
       <c r="C12">
         <f t="shared" si="1"/>
-        <v>141140400</v>
+        <v>6272635644000</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -3339,11 +3350,11 @@
       </c>
       <c r="B13">
         <f t="shared" si="0"/>
-        <v>52470600</v>
+        <v>5111954250000</v>
       </c>
       <c r="C13">
         <f t="shared" si="1"/>
-        <v>165642100</v>
+        <v>7975105281000</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -3352,11 +3363,11 @@
       </c>
       <c r="B14">
         <f t="shared" si="0"/>
-        <v>60846800</v>
+        <v>6384357000000</v>
       </c>
       <c r="C14">
         <f t="shared" si="1"/>
-        <v>192103800</v>
+        <v>9960714918000</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -3365,11 +3376,11 @@
       </c>
       <c r="B15">
         <f t="shared" si="0"/>
-        <v>69843000</v>
+        <v>7852106250000</v>
       </c>
       <c r="C15">
         <f t="shared" si="1"/>
-        <v>220525500</v>
+        <v>12251244555000</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -3378,11 +3389,11 @@
       </c>
       <c r="B16">
         <f t="shared" si="0"/>
-        <v>79459200</v>
+        <v>9529152000000</v>
       </c>
       <c r="C16">
         <f t="shared" si="1"/>
-        <v>250907200</v>
+        <v>14868474192000</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -3391,11 +3402,11 @@
       </c>
       <c r="B17">
         <f t="shared" si="0"/>
-        <v>89695400</v>
+        <v>11429444250000</v>
       </c>
       <c r="C17">
         <f t="shared" si="1"/>
-        <v>283248900</v>
+        <v>17834183829000</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -3404,11 +3415,11 @@
       </c>
       <c r="B18">
         <f t="shared" si="0"/>
-        <v>100551600</v>
+        <v>13566933000000</v>
       </c>
       <c r="C18">
         <f t="shared" si="1"/>
-        <v>317550600</v>
+        <v>21170153466000</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -3417,11 +3428,11 @@
       </c>
       <c r="B19">
         <f t="shared" si="0"/>
-        <v>112027800</v>
+        <v>15955568250000</v>
       </c>
       <c r="C19">
         <f t="shared" si="1"/>
-        <v>353812300</v>
+        <v>24898163103000</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -3430,11 +3441,11 @@
       </c>
       <c r="B20">
         <f t="shared" si="0"/>
-        <v>124124000</v>
+        <v>18609300000000</v>
       </c>
       <c r="C20">
         <f t="shared" si="1"/>
-        <v>392034000</v>
+        <v>29039992740000</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -3443,11 +3454,11 @@
       </c>
       <c r="B21">
         <f t="shared" si="0"/>
-        <v>136840200</v>
+        <v>21542078250000</v>
       </c>
       <c r="C21">
         <f t="shared" si="1"/>
-        <v>432215700</v>
+        <v>33617422377000</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -3456,11 +3467,11 @@
       </c>
       <c r="B22">
         <f t="shared" si="0"/>
-        <v>150176400</v>
+        <v>24767853000000</v>
       </c>
       <c r="C22">
         <f t="shared" si="1"/>
-        <v>474357400</v>
+        <v>38652232014000</v>
       </c>
     </row>
   </sheetData>
@@ -3473,8 +3484,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C22"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3507,12 +3518,12 @@
         <v>100</v>
       </c>
       <c r="B2">
-        <f xml:space="preserve"> A2 * (5 + 4*10 + 15 + 3*25 + A2*(2*5 + 10 + 20 + 25))</f>
-        <v>663500</v>
+        <f>A2*(4*10 + 5 + 3*15 +4*25)*(3*10 + 2*25 + 20 + 2*25)*((A2)*(A2+1))/2</f>
+        <v>14392500000</v>
       </c>
       <c r="C2">
-        <f>A2 * (2*10 + 5 + 20 + A2 * (2 * 5 + 3 * 10 + 6 * 25))</f>
-        <v>1904500</v>
+        <f xml:space="preserve"> A2 *(3*10+ 5 + 4*20)*(4*10 + 2*5 + 4*15 + 6*25)*((A2 - 1)*(A2 + 1))/2</f>
+        <v>14948505000</v>
       </c>
       <c r="H2" t="s">
         <v>5</v>
@@ -3526,12 +3537,12 @@
         <v>200</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:B22" si="0" xml:space="preserve"> A3 * (5 + 4*10 + 15 + 3*25 + A3*(2*5 + 10 + 20 + 25))</f>
-        <v>2627000</v>
+        <f t="shared" ref="B3:B22" si="0">A3*(4*10 + 5 + 3*15 +4*25)*(3*10 + 2*25 + 20 + 2*25)*((A3)*(A3+1))/2</f>
+        <v>114570000000</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C22" si="1">A3 * (2*10 + 5 + 20 + A3 * (2 * 5 + 3 * 10 + 6 * 25))</f>
-        <v>7609000</v>
+        <f t="shared" ref="C3:C22" si="1" xml:space="preserve"> A3 *(3*10+ 5 + 4*20)*(4*10 + 2*5 + 4*15 + 6*25)*((A3 - 1)*(A3 + 1))/2</f>
+        <v>119597010000</v>
       </c>
       <c r="H3" t="s">
         <v>3</v>
@@ -3546,11 +3557,11 @@
       </c>
       <c r="B4">
         <f t="shared" si="0"/>
-        <v>5890500</v>
+        <v>386032500000</v>
       </c>
       <c r="C4">
         <f t="shared" si="1"/>
-        <v>17113500</v>
+        <v>403645515000</v>
       </c>
       <c r="H4" t="s">
         <v>6</v>
@@ -3565,11 +3576,11 @@
       </c>
       <c r="B5">
         <f t="shared" si="0"/>
-        <v>10454000</v>
+        <v>914280000000</v>
       </c>
       <c r="C5">
         <f t="shared" si="1"/>
-        <v>30418000</v>
+        <v>956794020000</v>
       </c>
       <c r="H5" t="s">
         <v>7</v>
@@ -3584,11 +3595,11 @@
       </c>
       <c r="B6">
         <f t="shared" si="0"/>
-        <v>16317500</v>
+        <v>1784812500000</v>
       </c>
       <c r="C6">
         <f t="shared" si="1"/>
-        <v>47522500</v>
+        <v>1868742525000</v>
       </c>
       <c r="H6" t="s">
         <v>8</v>
@@ -3603,11 +3614,11 @@
       </c>
       <c r="B7">
         <f t="shared" si="0"/>
-        <v>23481000</v>
+        <v>3083130000000</v>
       </c>
       <c r="C7">
         <f t="shared" si="1"/>
-        <v>68427000</v>
+        <v>3229191030000</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -3616,11 +3627,11 @@
       </c>
       <c r="B8">
         <f t="shared" si="0"/>
-        <v>41708000</v>
+        <v>7305120000000</v>
       </c>
       <c r="C8">
         <f t="shared" si="1"/>
-        <v>121636000</v>
+        <v>7654388040000</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -3629,11 +3640,11 @@
       </c>
       <c r="B9">
         <f t="shared" si="0"/>
-        <v>52771500</v>
+        <v>10399792500000</v>
       </c>
       <c r="C9">
         <f t="shared" si="1"/>
-        <v>153940500</v>
+        <v>10898536545000</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -3642,11 +3653,11 @@
       </c>
       <c r="B10">
         <f t="shared" si="0"/>
-        <v>65135000</v>
+        <v>14264250000000</v>
       </c>
       <c r="C10">
         <f t="shared" si="1"/>
-        <v>190045000</v>
+        <v>14949985050000</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -3655,11 +3666,11 @@
       </c>
       <c r="B11">
         <f t="shared" si="0"/>
-        <v>78798500</v>
+        <v>18983992500000</v>
       </c>
       <c r="C11">
         <f t="shared" si="1"/>
-        <v>229949500</v>
+        <v>19898433555000</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -3668,11 +3679,11 @@
       </c>
       <c r="B12">
         <f t="shared" si="0"/>
-        <v>93762000</v>
+        <v>24644520000000</v>
       </c>
       <c r="C12">
         <f t="shared" si="1"/>
-        <v>273654000</v>
+        <v>25833582060000</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -3681,11 +3692,11 @@
       </c>
       <c r="B13">
         <f t="shared" si="0"/>
-        <v>110025500</v>
+        <v>31331332500000</v>
       </c>
       <c r="C13">
         <f t="shared" si="1"/>
-        <v>321158500</v>
+        <v>32845130565000</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -3694,11 +3705,11 @@
       </c>
       <c r="B14">
         <f t="shared" si="0"/>
-        <v>127589000</v>
+        <v>39129930000000</v>
       </c>
       <c r="C14">
         <f t="shared" si="1"/>
-        <v>372463000</v>
+        <v>41022779070000</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -3707,11 +3718,11 @@
       </c>
       <c r="B15">
         <f t="shared" si="0"/>
-        <v>146452500</v>
+        <v>48125812500000</v>
       </c>
       <c r="C15">
         <f t="shared" si="1"/>
-        <v>427567500</v>
+        <v>50456227575000</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -3720,11 +3731,11 @@
       </c>
       <c r="B16">
         <f t="shared" si="0"/>
-        <v>166616000</v>
+        <v>58404480000000</v>
       </c>
       <c r="C16">
         <f t="shared" si="1"/>
-        <v>486472000</v>
+        <v>61235176080000</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -3733,11 +3744,11 @@
       </c>
       <c r="B17">
         <f t="shared" si="0"/>
-        <v>188079500</v>
+        <v>70051432500000</v>
       </c>
       <c r="C17">
         <f t="shared" si="1"/>
-        <v>549176500</v>
+        <v>73449324585000</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -3746,11 +3757,11 @@
       </c>
       <c r="B18">
         <f t="shared" si="0"/>
-        <v>210843000</v>
+        <v>83152170000000</v>
       </c>
       <c r="C18">
         <f t="shared" si="1"/>
-        <v>615681000</v>
+        <v>87188373090000</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -3759,11 +3770,11 @@
       </c>
       <c r="B19">
         <f t="shared" si="0"/>
-        <v>234906500</v>
+        <v>97792192500000</v>
       </c>
       <c r="C19">
         <f t="shared" si="1"/>
-        <v>685985500</v>
+        <v>102542021595000</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -3772,11 +3783,11 @@
       </c>
       <c r="B20">
         <f t="shared" si="0"/>
-        <v>260270000</v>
+        <v>114057000000000</v>
       </c>
       <c r="C20">
         <f t="shared" si="1"/>
-        <v>760090000</v>
+        <v>119599970100000</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -3785,11 +3796,11 @@
       </c>
       <c r="B21">
         <f t="shared" si="0"/>
-        <v>286933500</v>
+        <v>132032092500000</v>
       </c>
       <c r="C21">
         <f t="shared" si="1"/>
-        <v>837994500</v>
+        <v>138451918605000</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -3798,11 +3809,11 @@
       </c>
       <c r="B22">
         <f t="shared" si="0"/>
-        <v>314897000</v>
+        <v>151802970000000</v>
       </c>
       <c r="C22">
         <f t="shared" si="1"/>
-        <v>919699000</v>
+        <v>159187567110000</v>
       </c>
     </row>
   </sheetData>
@@ -3815,8 +3826,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3848,12 +3859,12 @@
         <v>100</v>
       </c>
       <c r="B2">
-        <f xml:space="preserve"> A2 * (2 + 4*10 + 6 + 3*10 + A2*(2*2 + 4 + 8 + 10))</f>
-        <v>267800</v>
+        <f>A2*(4*4 + 2 + 3*6 +4*10)*(3*4 + 2*2 + 8 + 2*10)*((A2)*(A2+1))/2</f>
+        <v>1688720000</v>
       </c>
       <c r="C2">
-        <f>A2 * (2*4 + 2 + 8 + A2 * (2 * 2 + 3 * 4 + 6 * 10))</f>
-        <v>761800</v>
+        <f xml:space="preserve"> A2 *(3*4 + 2 + 4*8)*(4*4 + 2*2 + 4*6 + 6*10)*((A2 - 1)*(A2 + 1))/2</f>
+        <v>2391760800</v>
       </c>
       <c r="H2" t="s">
         <v>5</v>
@@ -3867,12 +3878,12 @@
         <v>200</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:B22" si="0" xml:space="preserve"> A3 * (2 + 4*10 + 6 + 3*10 + A3*(2*2 + 4 + 8 + 10))</f>
-        <v>1055600</v>
+        <f t="shared" ref="B3:B22" si="0">A3*(4*4 + 2 + 3*6 +4*10)*(3*4 + 2*2 + 8 + 2*10)*((A3)*(A3+1))/2</f>
+        <v>13442880000</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C22" si="1">A3 * (2*4 + 2 + 8 + A3 * (2 * 2 + 3 * 4 + 6 * 10))</f>
-        <v>3043600</v>
+        <f t="shared" ref="C3:C22" si="1" xml:space="preserve"> A3 *(3*4 + 2 + 4*8)*(4*4 + 2*2 + 4*6 + 6*10)*((A3 - 1)*(A3 + 1))/2</f>
+        <v>19135521600</v>
       </c>
       <c r="H3" t="s">
         <v>3</v>
@@ -3887,11 +3898,11 @@
       </c>
       <c r="B4">
         <f t="shared" si="0"/>
-        <v>2363400</v>
+        <v>45294480000</v>
       </c>
       <c r="C4">
         <f t="shared" si="1"/>
-        <v>6845400</v>
+        <v>64583282400</v>
       </c>
       <c r="H4" t="s">
         <v>6</v>
@@ -3906,11 +3917,11 @@
       </c>
       <c r="B5">
         <f t="shared" si="0"/>
-        <v>4191200</v>
+        <v>107275520000</v>
       </c>
       <c r="C5">
         <f t="shared" si="1"/>
-        <v>12167200</v>
+        <v>153087043200</v>
       </c>
       <c r="H5" t="s">
         <v>7</v>
@@ -3925,11 +3936,11 @@
       </c>
       <c r="B6">
         <f t="shared" si="0"/>
-        <v>6539000</v>
+        <v>209418000000</v>
       </c>
       <c r="C6">
         <f t="shared" si="1"/>
-        <v>19009000</v>
+        <v>298998804000</v>
       </c>
       <c r="H6" t="s">
         <v>8</v>
@@ -3944,11 +3955,11 @@
       </c>
       <c r="B7">
         <f t="shared" si="0"/>
-        <v>9406800</v>
+        <v>361753920000</v>
       </c>
       <c r="C7">
         <f t="shared" si="1"/>
-        <v>27370800</v>
+        <v>516670564800</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -3957,11 +3968,11 @@
       </c>
       <c r="B8">
         <f t="shared" si="0"/>
-        <v>16702400</v>
+        <v>857134080000</v>
       </c>
       <c r="C8">
         <f t="shared" si="1"/>
-        <v>48654400</v>
+        <v>1224702086400</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -3970,11 +3981,11 @@
       </c>
       <c r="B9">
         <f t="shared" si="0"/>
-        <v>21130200</v>
+        <v>1220242320000</v>
       </c>
       <c r="C9">
         <f t="shared" si="1"/>
-        <v>61576200</v>
+        <v>1743765847200</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -3983,11 +3994,11 @@
       </c>
       <c r="B10">
         <f t="shared" si="0"/>
-        <v>26078000</v>
+        <v>1673672000000</v>
       </c>
       <c r="C10">
         <f t="shared" si="1"/>
-        <v>76018000</v>
+        <v>2391997608000</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -3996,11 +4007,11 @@
       </c>
       <c r="B11">
         <f t="shared" si="0"/>
-        <v>31545800</v>
+        <v>2227455120000</v>
       </c>
       <c r="C11">
         <f t="shared" si="1"/>
-        <v>91979800</v>
+        <v>3183749368800</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -4009,11 +4020,11 @@
       </c>
       <c r="B12">
         <f t="shared" si="0"/>
-        <v>37533600</v>
+        <v>2891623680000</v>
       </c>
       <c r="C12">
         <f t="shared" si="1"/>
-        <v>109461600</v>
+        <v>4133373129600</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -4022,11 +4033,11 @@
       </c>
       <c r="B13">
         <f t="shared" si="0"/>
-        <v>44041400</v>
+        <v>3676209680000</v>
       </c>
       <c r="C13">
         <f t="shared" si="1"/>
-        <v>128463400</v>
+        <v>5255220890400</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -4035,11 +4046,11 @@
       </c>
       <c r="B14">
         <f t="shared" si="0"/>
-        <v>51069200</v>
+        <v>4591245120000</v>
       </c>
       <c r="C14">
         <f t="shared" si="1"/>
-        <v>148985200</v>
+        <v>6563644651200</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -4048,11 +4059,11 @@
       </c>
       <c r="B15">
         <f t="shared" si="0"/>
-        <v>58617000</v>
+        <v>5646762000000</v>
       </c>
       <c r="C15">
         <f t="shared" si="1"/>
-        <v>171027000</v>
+        <v>8072996412000</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -4061,11 +4072,11 @@
       </c>
       <c r="B16">
         <f t="shared" si="0"/>
-        <v>66684800</v>
+        <v>6852792320000</v>
       </c>
       <c r="C16">
         <f t="shared" si="1"/>
-        <v>194588800</v>
+        <v>9797628172800</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -4074,11 +4085,11 @@
       </c>
       <c r="B17">
         <f t="shared" si="0"/>
-        <v>75272600</v>
+        <v>8219368080000</v>
       </c>
       <c r="C17">
         <f t="shared" si="1"/>
-        <v>219670600</v>
+        <v>11751891933600</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -4087,11 +4098,11 @@
       </c>
       <c r="B18">
         <f t="shared" si="0"/>
-        <v>84380400</v>
+        <v>9756521280000</v>
       </c>
       <c r="C18">
         <f t="shared" si="1"/>
-        <v>246272400</v>
+        <v>13950139694400</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -4100,11 +4111,11 @@
       </c>
       <c r="B19">
         <f t="shared" si="0"/>
-        <v>94008200</v>
+        <v>11474283920000</v>
       </c>
       <c r="C19">
         <f t="shared" si="1"/>
-        <v>274394200</v>
+        <v>16406723455200</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -4113,11 +4124,11 @@
       </c>
       <c r="B20">
         <f t="shared" si="0"/>
-        <v>104156000</v>
+        <v>13382688000000</v>
       </c>
       <c r="C20">
         <f t="shared" si="1"/>
-        <v>304036000</v>
+        <v>19135995216000</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -4126,11 +4137,11 @@
       </c>
       <c r="B21">
         <f t="shared" si="0"/>
-        <v>114823800</v>
+        <v>15491765520000</v>
       </c>
       <c r="C21">
         <f t="shared" si="1"/>
-        <v>335197800</v>
+        <v>22152306976800</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -4139,11 +4150,11 @@
       </c>
       <c r="B22">
         <f t="shared" si="0"/>
-        <v>126011600</v>
+        <v>17811548480000</v>
       </c>
       <c r="C22">
         <f t="shared" si="1"/>
-        <v>367879600</v>
+        <v>25470010737600</v>
       </c>
     </row>
   </sheetData>
@@ -4156,8 +4167,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="T33" sqref="T33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4190,12 +4201,12 @@
         <v>100</v>
       </c>
       <c r="B2">
-        <f xml:space="preserve"> A2 * (3 + 4*6 + 9 + 3*15 + A2*(2*3 + 6 + 12 + 15))</f>
-        <v>398100</v>
+        <f>A2*(4*6 + 3 + 3*9 +4*15)*(3*6 + 2*3 + 12 + 2*15)*((A2)*(A2+1))/2</f>
+        <v>3799620000</v>
       </c>
       <c r="C2">
-        <f>A2 * (2*6 + 3 + 9 + A2 * (2 * 3 + 3 * 6 + 6 * 15))</f>
-        <v>1142400</v>
+        <f xml:space="preserve"> A2 *(3*6 + 3 + 4*12)*(4*6 + 2*3 + 4*9 + 6*15)*((A2 - 1)*(A2 + 1))/2</f>
+        <v>5381461800</v>
       </c>
       <c r="H2" t="s">
         <v>5</v>
@@ -4209,12 +4220,12 @@
         <v>200</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:B22" si="0" xml:space="preserve"> A3 * (3 + 4*6 + 9 + 3*15 + A3*(2*3 + 6 + 12 + 15))</f>
-        <v>1576200</v>
+        <f t="shared" ref="B3:B22" si="0">A3*(4*6 + 3 + 3*9 +4*15)*(3*6 + 2*3 + 12 + 2*15)*((A3)*(A3+1))/2</f>
+        <v>30246480000</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C22" si="1">A3 * (2*6 + 3 + 9 + A3 * (2 * 3 + 3 * 6 + 6 * 15))</f>
-        <v>4564800</v>
+        <f t="shared" ref="C3:C22" si="1" xml:space="preserve"> A3 *(3*6 + 3 + 4*12)*(4*6 + 2*3 + 4*9 + 6*15)*((A3 - 1)*(A3 + 1))/2</f>
+        <v>43054923600</v>
       </c>
       <c r="H3" t="s">
         <v>3</v>
@@ -4229,11 +4240,11 @@
       </c>
       <c r="B4">
         <f t="shared" si="0"/>
-        <v>3534300</v>
+        <v>101912580000</v>
       </c>
       <c r="C4">
         <f t="shared" si="1"/>
-        <v>10267200</v>
+        <v>145312385400</v>
       </c>
       <c r="H4" t="s">
         <v>6</v>
@@ -4248,11 +4259,11 @@
       </c>
       <c r="B5">
         <f t="shared" si="0"/>
-        <v>6272400</v>
+        <v>241369920000</v>
       </c>
       <c r="C5">
         <f t="shared" si="1"/>
-        <v>18249600</v>
+        <v>344445847200</v>
       </c>
       <c r="H5" t="s">
         <v>7</v>
@@ -4267,11 +4278,11 @@
       </c>
       <c r="B6">
         <f t="shared" si="0"/>
-        <v>9790500</v>
+        <v>471190500000</v>
       </c>
       <c r="C6">
         <f t="shared" si="1"/>
-        <v>28512000</v>
+        <v>672747309000</v>
       </c>
       <c r="H6" t="s">
         <v>8</v>
@@ -4286,11 +4297,11 @@
       </c>
       <c r="B7">
         <f t="shared" si="0"/>
-        <v>14088600</v>
+        <v>813946320000</v>
       </c>
       <c r="C7">
         <f t="shared" si="1"/>
-        <v>41054400</v>
+        <v>1162508770800</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -4299,11 +4310,11 @@
       </c>
       <c r="B8">
         <f t="shared" si="0"/>
-        <v>25024800</v>
+        <v>1928551680000</v>
       </c>
       <c r="C8">
         <f t="shared" si="1"/>
-        <v>72979200</v>
+        <v>2755579694400</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -4312,11 +4323,11 @@
       </c>
       <c r="B9">
         <f t="shared" si="0"/>
-        <v>31662900</v>
+        <v>2745545220000</v>
       </c>
       <c r="C9">
         <f t="shared" si="1"/>
-        <v>92361600</v>
+        <v>3923473156200</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -4325,11 +4336,11 @@
       </c>
       <c r="B10">
         <f t="shared" si="0"/>
-        <v>39081000</v>
+        <v>3765762000000</v>
       </c>
       <c r="C10">
         <f t="shared" si="1"/>
-        <v>114024000</v>
+        <v>5381994618000</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -4338,11 +4349,11 @@
       </c>
       <c r="B11">
         <f t="shared" si="0"/>
-        <v>47279100</v>
+        <v>5011774020000</v>
       </c>
       <c r="C11">
         <f t="shared" si="1"/>
-        <v>137966400</v>
+        <v>7163436079800</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -4351,11 +4362,11 @@
       </c>
       <c r="B12">
         <f t="shared" si="0"/>
-        <v>56257200</v>
+        <v>6506153280000</v>
       </c>
       <c r="C12">
         <f t="shared" si="1"/>
-        <v>164188800</v>
+        <v>9300089541600</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -4364,11 +4375,11 @@
       </c>
       <c r="B13">
         <f t="shared" si="0"/>
-        <v>66015300</v>
+        <v>8271471780000</v>
       </c>
       <c r="C13">
         <f t="shared" si="1"/>
-        <v>192691200</v>
+        <v>11824247003400</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -4377,11 +4388,11 @@
       </c>
       <c r="B14">
         <f t="shared" si="0"/>
-        <v>76553400</v>
+        <v>10330301520000</v>
       </c>
       <c r="C14">
         <f t="shared" si="1"/>
-        <v>223473600</v>
+        <v>14768200465200</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -4390,11 +4401,11 @@
       </c>
       <c r="B15">
         <f t="shared" si="0"/>
-        <v>87871500</v>
+        <v>12705214500000</v>
       </c>
       <c r="C15">
         <f t="shared" si="1"/>
-        <v>256536000</v>
+        <v>18164241927000</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -4403,11 +4414,11 @@
       </c>
       <c r="B16">
         <f t="shared" si="0"/>
-        <v>99969600</v>
+        <v>15418782720000</v>
       </c>
       <c r="C16">
         <f t="shared" si="1"/>
-        <v>291878400</v>
+        <v>22044663388800</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -4416,11 +4427,11 @@
       </c>
       <c r="B17">
         <f t="shared" si="0"/>
-        <v>112847700</v>
+        <v>18493578180000</v>
       </c>
       <c r="C17">
         <f t="shared" si="1"/>
-        <v>329500800</v>
+        <v>26441756850600</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -4429,11 +4440,11 @@
       </c>
       <c r="B18">
         <f t="shared" si="0"/>
-        <v>126505800</v>
+        <v>21952172880000</v>
       </c>
       <c r="C18">
         <f t="shared" si="1"/>
-        <v>369403200</v>
+        <v>31387814312400</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -4442,11 +4453,11 @@
       </c>
       <c r="B19">
         <f t="shared" si="0"/>
-        <v>140943900</v>
+        <v>25817138820000</v>
       </c>
       <c r="C19">
         <f t="shared" si="1"/>
-        <v>411585600</v>
+        <v>36915127774200</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -4455,11 +4466,11 @@
       </c>
       <c r="B20">
         <f t="shared" si="0"/>
-        <v>156162000</v>
+        <v>30111048000000</v>
       </c>
       <c r="C20">
         <f t="shared" si="1"/>
-        <v>456048000</v>
+        <v>43055989236000</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -4468,11 +4479,11 @@
       </c>
       <c r="B21">
         <f t="shared" si="0"/>
-        <v>172160100</v>
+        <v>34856472420000</v>
       </c>
       <c r="C21">
         <f t="shared" si="1"/>
-        <v>502790400</v>
+        <v>49842690697800</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -4481,11 +4492,11 @@
       </c>
       <c r="B22">
         <f t="shared" si="0"/>
-        <v>188938200</v>
+        <v>40075984080000</v>
       </c>
       <c r="C22">
         <f t="shared" si="1"/>
-        <v>551812800</v>
+        <v>57307524159600</v>
       </c>
     </row>
   </sheetData>

</xml_diff>